<commit_message>
Add whisper and lobby chat
</commit_message>
<xml_diff>
--- a/ChatProgram/시퀸스 다이얼그램.xlsx
+++ b/ChatProgram/시퀸스 다이얼그램.xlsx
@@ -5,22 +5,25 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\00_Dev\Github_gameServerLessonsCodes\trunk\Demo08-1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Practice\GameServerProgramming\ChatProgram\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21345" windowHeight="11715" tabRatio="683" firstSheet="2" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21345" windowHeight="11715" tabRatio="683" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="로그인" sheetId="1" r:id="rId1"/>
     <sheet name="로비 리스트 요청" sheetId="2" r:id="rId2"/>
-    <sheet name="로비 들어가기" sheetId="3" r:id="rId3"/>
-    <sheet name="로비-방리스트 요청" sheetId="8" r:id="rId4"/>
-    <sheet name="로비-유저 리스트 요청" sheetId="10" r:id="rId5"/>
-    <sheet name="로비 나가기" sheetId="4" r:id="rId6"/>
-    <sheet name="방 입장" sheetId="5" r:id="rId7"/>
-    <sheet name="방 나가기" sheetId="6" r:id="rId8"/>
-    <sheet name="방 채팅" sheetId="7" r:id="rId9"/>
+    <sheet name="로비 채팅" sheetId="13" r:id="rId3"/>
+    <sheet name="로비 들어가기" sheetId="3" r:id="rId4"/>
+    <sheet name="로비-방리스트 요청" sheetId="8" r:id="rId5"/>
+    <sheet name="로비-유저 리스트 요청" sheetId="10" r:id="rId6"/>
+    <sheet name="Sheet1" sheetId="11" r:id="rId7"/>
+    <sheet name="Sheet2" sheetId="12" r:id="rId8"/>
+    <sheet name="로비 나가기" sheetId="4" r:id="rId9"/>
+    <sheet name="방 입장" sheetId="5" r:id="rId10"/>
+    <sheet name="방 나가기" sheetId="6" r:id="rId11"/>
+    <sheet name="방 채팅" sheetId="7" r:id="rId12"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -80,8 +83,36 @@
   <cellStyles count="1">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1253,6 +1284,1480 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing10.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>19053</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>61913</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>90490</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>172613</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="14" name="Rectangle 5"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="1390653" y="1319213"/>
+          <a:ext cx="71437" cy="1368000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent1"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr wrap="square" anchor="ctr"/>
+        <a:lstStyle>
+          <a:defPPr>
+            <a:defRPr lang="ko-KR"/>
+          </a:defPPr>
+          <a:lvl1pPr marL="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p>
+          <a:endParaRPr lang="ko-KR" altLang="en-US"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>309590</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>101606</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>450877</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>198446</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="15" name="Group 7"/>
+        <xdr:cNvGrpSpPr>
+          <a:grpSpLocks/>
+        </xdr:cNvGrpSpPr>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="3738590" y="311156"/>
+          <a:ext cx="1512887" cy="935040"/>
+          <a:chOff x="427" y="270"/>
+          <a:chExt cx="91" cy="96"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="16" name="Text Box 8"/>
+          <xdr:cNvSpPr txBox="1">
+            <a:spLocks noChangeArrowheads="1"/>
+          </xdr:cNvSpPr>
+        </xdr:nvSpPr>
+        <xdr:spPr bwMode="auto">
+          <a:xfrm>
+            <a:off x="429" y="345"/>
+            <a:ext cx="89" cy="21"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:srgbClr val="FFFFFF"/>
+          </a:solidFill>
+          <a:ln w="9525">
+            <a:noFill/>
+            <a:miter lim="800000"/>
+            <a:headEnd/>
+            <a:tailEnd/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:txBody>
+          <a:bodyPr wrap="square"/>
+          <a:lstStyle>
+            <a:defPPr>
+              <a:defRPr lang="ko-KR"/>
+            </a:defPPr>
+            <a:lvl1pPr marL="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl1pPr>
+            <a:lvl2pPr marL="457200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl2pPr>
+            <a:lvl3pPr marL="914400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl3pPr>
+            <a:lvl4pPr marL="1371600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl4pPr>
+            <a:lvl5pPr marL="1828800" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl5pPr>
+            <a:lvl6pPr marL="2286000" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl6pPr>
+            <a:lvl7pPr marL="2743200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl7pPr>
+            <a:lvl8pPr marL="3200400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl8pPr>
+            <a:lvl9pPr marL="3657600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl9pPr>
+          </a:lstStyle>
+          <a:p>
+            <a:r>
+              <a:rPr lang="en-US" altLang="ko-KR" sz="1200"/>
+              <a:t>   </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="ko-KR" altLang="en-US" sz="1200"/>
+              <a:t>채팅 서버</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:pic>
+        <xdr:nvPicPr>
+          <xdr:cNvPr id="17" name="Picture 9"/>
+          <xdr:cNvPicPr>
+            <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+          </xdr:cNvPicPr>
+        </xdr:nvPicPr>
+        <xdr:blipFill>
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+          <a:srcRect/>
+          <a:stretch>
+            <a:fillRect/>
+          </a:stretch>
+        </xdr:blipFill>
+        <xdr:spPr bwMode="auto">
+          <a:xfrm>
+            <a:off x="427" y="270"/>
+            <a:ext cx="78" cy="78"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln w="9525">
+            <a:noFill/>
+            <a:miter lim="800000"/>
+            <a:headEnd/>
+            <a:tailEnd/>
+          </a:ln>
+        </xdr:spPr>
+      </xdr:pic>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>104776</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>107941</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>178596</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="18" name="Text Box 10"/>
+        <xdr:cNvSpPr txBox="1">
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="2847976" y="1574791"/>
+          <a:ext cx="1495424" cy="280205"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525">
+          <a:noFill/>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr wrap="square">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle>
+          <a:defPPr>
+            <a:defRPr lang="ko-KR"/>
+          </a:defPPr>
+          <a:lvl1pPr marL="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p>
+          <a:pPr>
+            <a:spcBef>
+              <a:spcPct val="50000"/>
+            </a:spcBef>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ko-KR" sz="1200"/>
+            <a:t>ROOM_CHAT_REQ</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>276225</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>669925</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="19" name="Group 4"/>
+        <xdr:cNvGrpSpPr>
+          <a:grpSpLocks/>
+        </xdr:cNvGrpSpPr>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="962025" y="295275"/>
+          <a:ext cx="1079500" cy="1025525"/>
+          <a:chOff x="1247" y="2976"/>
+          <a:chExt cx="680" cy="646"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:pic>
+        <xdr:nvPicPr>
+          <xdr:cNvPr id="20" name="Picture 5"/>
+          <xdr:cNvPicPr>
+            <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+          </xdr:cNvPicPr>
+        </xdr:nvPicPr>
+        <xdr:blipFill>
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+          <a:srcRect/>
+          <a:stretch>
+            <a:fillRect/>
+          </a:stretch>
+        </xdr:blipFill>
+        <xdr:spPr bwMode="auto">
+          <a:xfrm>
+            <a:off x="1338" y="2976"/>
+            <a:ext cx="456" cy="462"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln w="9525">
+            <a:noFill/>
+            <a:miter lim="800000"/>
+            <a:headEnd/>
+            <a:tailEnd/>
+          </a:ln>
+        </xdr:spPr>
+      </xdr:pic>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="21" name="Text Box 6"/>
+          <xdr:cNvSpPr txBox="1">
+            <a:spLocks noChangeArrowheads="1"/>
+          </xdr:cNvSpPr>
+        </xdr:nvSpPr>
+        <xdr:spPr bwMode="auto">
+          <a:xfrm>
+            <a:off x="1247" y="3430"/>
+            <a:ext cx="680" cy="192"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln w="9525">
+            <a:noFill/>
+            <a:miter lim="800000"/>
+            <a:headEnd/>
+            <a:tailEnd/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:txBody>
+          <a:bodyPr wrap="square">
+            <a:spAutoFit/>
+          </a:bodyPr>
+          <a:lstStyle>
+            <a:defPPr>
+              <a:defRPr lang="ko-KR"/>
+            </a:defPPr>
+            <a:lvl1pPr marL="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl1pPr>
+            <a:lvl2pPr marL="457200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl2pPr>
+            <a:lvl3pPr marL="914400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl3pPr>
+            <a:lvl4pPr marL="1371600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl4pPr>
+            <a:lvl5pPr marL="1828800" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl5pPr>
+            <a:lvl6pPr marL="2286000" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl6pPr>
+            <a:lvl7pPr marL="2743200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl7pPr>
+            <a:lvl8pPr marL="3200400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl8pPr>
+            <a:lvl9pPr marL="3657600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl9pPr>
+          </a:lstStyle>
+          <a:p>
+            <a:pPr>
+              <a:spcBef>
+                <a:spcPct val="50000"/>
+              </a:spcBef>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="ko-KR" altLang="en-US" sz="1400"/>
+              <a:t>클라이언트</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>195294</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>61912</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>266732</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>132862</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="22" name="Rectangle 5"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="4310094" y="1319212"/>
+          <a:ext cx="71438" cy="2376000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent1"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr wrap="square" anchor="ctr"/>
+        <a:lstStyle>
+          <a:defPPr>
+            <a:defRPr lang="ko-KR"/>
+          </a:defPPr>
+          <a:lvl1pPr marL="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p>
+          <a:endParaRPr lang="ko-KR" altLang="en-US"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>90490</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>153980</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>161924</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>153980</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="23" name="직선 화살표 연결선 22"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1462090" y="1830380"/>
+          <a:ext cx="2814634" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>90490</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>93662</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>180974</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>93662</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="24" name="직선 화살표 연결선 23"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="1462090" y="2398712"/>
+          <a:ext cx="2833684" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>161925</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>26213</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>200024</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>96868</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="25" name="Text Box 10"/>
+        <xdr:cNvSpPr txBox="1">
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="1533525" y="2121713"/>
+          <a:ext cx="1409699" cy="280205"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525">
+          <a:noFill/>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr wrap="square">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle>
+          <a:defPPr>
+            <a:defRPr lang="ko-KR"/>
+          </a:defPPr>
+          <a:lvl1pPr marL="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p>
+          <a:pPr>
+            <a:spcBef>
+              <a:spcPct val="50000"/>
+            </a:spcBef>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ko-KR" sz="1200"/>
+            <a:t>ROOM_CHAT_RES</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="26" name="Group 4"/>
+        <xdr:cNvGrpSpPr>
+          <a:grpSpLocks/>
+        </xdr:cNvGrpSpPr>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="2667000"/>
+          <a:ext cx="1600200" cy="1123950"/>
+          <a:chOff x="1037" y="2976"/>
+          <a:chExt cx="1008" cy="708"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:pic>
+        <xdr:nvPicPr>
+          <xdr:cNvPr id="27" name="Picture 5"/>
+          <xdr:cNvPicPr>
+            <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+          </xdr:cNvPicPr>
+        </xdr:nvPicPr>
+        <xdr:blipFill>
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+          <a:srcRect/>
+          <a:stretch>
+            <a:fillRect/>
+          </a:stretch>
+        </xdr:blipFill>
+        <xdr:spPr bwMode="auto">
+          <a:xfrm>
+            <a:off x="1338" y="2976"/>
+            <a:ext cx="456" cy="462"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln w="9525">
+            <a:noFill/>
+            <a:miter lim="800000"/>
+            <a:headEnd/>
+            <a:tailEnd/>
+          </a:ln>
+        </xdr:spPr>
+      </xdr:pic>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="28" name="Text Box 6"/>
+          <xdr:cNvSpPr txBox="1">
+            <a:spLocks noChangeArrowheads="1"/>
+          </xdr:cNvSpPr>
+        </xdr:nvSpPr>
+        <xdr:spPr bwMode="auto">
+          <a:xfrm>
+            <a:off x="1037" y="3430"/>
+            <a:ext cx="1008" cy="254"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln w="9525">
+            <a:noFill/>
+            <a:miter lim="800000"/>
+            <a:headEnd/>
+            <a:tailEnd/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:txBody>
+          <a:bodyPr wrap="square">
+            <a:spAutoFit/>
+          </a:bodyPr>
+          <a:lstStyle>
+            <a:defPPr>
+              <a:defRPr lang="ko-KR"/>
+            </a:defPPr>
+            <a:lvl1pPr marL="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl1pPr>
+            <a:lvl2pPr marL="457200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl2pPr>
+            <a:lvl3pPr marL="914400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl3pPr>
+            <a:lvl4pPr marL="1371600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl4pPr>
+            <a:lvl5pPr marL="1828800" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl5pPr>
+            <a:lvl6pPr marL="2286000" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl6pPr>
+            <a:lvl7pPr marL="2743200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl7pPr>
+            <a:lvl8pPr marL="3200400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl8pPr>
+            <a:lvl9pPr marL="3657600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl9pPr>
+          </a:lstStyle>
+          <a:p>
+            <a:pPr>
+              <a:spcBef>
+                <a:spcPct val="50000"/>
+              </a:spcBef>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="ko-KR" altLang="en-US" sz="1400"/>
+              <a:t>방의 다른 유저</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>609600</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>774</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>195259</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>774</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="29" name="직선 화살표 연결선 28"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="1295400" y="3353574"/>
+          <a:ext cx="3014659" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>52385</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>90484</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>3980</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="30" name="Text Box 10"/>
+        <xdr:cNvSpPr txBox="1">
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="1423985" y="3076575"/>
+          <a:ext cx="1409699" cy="280205"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525">
+          <a:noFill/>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr wrap="square">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle>
+          <a:defPPr>
+            <a:defRPr lang="ko-KR"/>
+          </a:defPPr>
+          <a:lvl1pPr marL="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p>
+          <a:pPr>
+            <a:spcBef>
+              <a:spcPct val="50000"/>
+            </a:spcBef>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ko-KR" sz="1200"/>
+            <a:t>ROOM_CHAT_NTF</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -2338,6 +3843,1480 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>2</xdr:col>
+      <xdr:colOff>19053</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>61913</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>90490</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>172613</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Rectangle 5"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="1390653" y="1319213"/>
+          <a:ext cx="71437" cy="1368000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent1"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr wrap="square" anchor="ctr"/>
+        <a:lstStyle>
+          <a:defPPr>
+            <a:defRPr lang="ko-KR"/>
+          </a:defPPr>
+          <a:lvl1pPr marL="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p>
+          <a:endParaRPr lang="ko-KR" altLang="en-US"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>309590</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>101606</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>450877</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>198446</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="3" name="Group 7"/>
+        <xdr:cNvGrpSpPr>
+          <a:grpSpLocks/>
+        </xdr:cNvGrpSpPr>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="3738590" y="311156"/>
+          <a:ext cx="1512887" cy="935040"/>
+          <a:chOff x="427" y="270"/>
+          <a:chExt cx="91" cy="96"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="4" name="Text Box 8"/>
+          <xdr:cNvSpPr txBox="1">
+            <a:spLocks noChangeArrowheads="1"/>
+          </xdr:cNvSpPr>
+        </xdr:nvSpPr>
+        <xdr:spPr bwMode="auto">
+          <a:xfrm>
+            <a:off x="429" y="345"/>
+            <a:ext cx="89" cy="21"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:srgbClr val="FFFFFF"/>
+          </a:solidFill>
+          <a:ln w="9525">
+            <a:noFill/>
+            <a:miter lim="800000"/>
+            <a:headEnd/>
+            <a:tailEnd/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:txBody>
+          <a:bodyPr wrap="square"/>
+          <a:lstStyle>
+            <a:defPPr>
+              <a:defRPr lang="ko-KR"/>
+            </a:defPPr>
+            <a:lvl1pPr marL="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl1pPr>
+            <a:lvl2pPr marL="457200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl2pPr>
+            <a:lvl3pPr marL="914400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl3pPr>
+            <a:lvl4pPr marL="1371600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl4pPr>
+            <a:lvl5pPr marL="1828800" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl5pPr>
+            <a:lvl6pPr marL="2286000" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl6pPr>
+            <a:lvl7pPr marL="2743200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl7pPr>
+            <a:lvl8pPr marL="3200400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl8pPr>
+            <a:lvl9pPr marL="3657600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl9pPr>
+          </a:lstStyle>
+          <a:p>
+            <a:r>
+              <a:rPr lang="en-US" altLang="ko-KR" sz="1200"/>
+              <a:t>   </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="ko-KR" altLang="en-US" sz="1200"/>
+              <a:t>채팅 서버</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:pic>
+        <xdr:nvPicPr>
+          <xdr:cNvPr id="5" name="Picture 9"/>
+          <xdr:cNvPicPr>
+            <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+          </xdr:cNvPicPr>
+        </xdr:nvPicPr>
+        <xdr:blipFill>
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+          <a:srcRect/>
+          <a:stretch>
+            <a:fillRect/>
+          </a:stretch>
+        </xdr:blipFill>
+        <xdr:spPr bwMode="auto">
+          <a:xfrm>
+            <a:off x="427" y="270"/>
+            <a:ext cx="78" cy="78"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln w="9525">
+            <a:noFill/>
+            <a:miter lim="800000"/>
+            <a:headEnd/>
+            <a:tailEnd/>
+          </a:ln>
+        </xdr:spPr>
+      </xdr:pic>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>104776</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>107941</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>178596</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="6" name="Text Box 10"/>
+        <xdr:cNvSpPr txBox="1">
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="2847976" y="1574791"/>
+          <a:ext cx="1495424" cy="280205"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525">
+          <a:noFill/>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr wrap="square">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle>
+          <a:defPPr>
+            <a:defRPr lang="ko-KR"/>
+          </a:defPPr>
+          <a:lvl1pPr marL="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p>
+          <a:pPr>
+            <a:spcBef>
+              <a:spcPct val="50000"/>
+            </a:spcBef>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ko-KR" sz="1200"/>
+            <a:t>LOBBY_CHAT_REQ</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>276225</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>669925</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="7" name="Group 4"/>
+        <xdr:cNvGrpSpPr>
+          <a:grpSpLocks/>
+        </xdr:cNvGrpSpPr>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="962025" y="295275"/>
+          <a:ext cx="1079500" cy="1025525"/>
+          <a:chOff x="1247" y="2976"/>
+          <a:chExt cx="680" cy="646"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:pic>
+        <xdr:nvPicPr>
+          <xdr:cNvPr id="8" name="Picture 5"/>
+          <xdr:cNvPicPr>
+            <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+          </xdr:cNvPicPr>
+        </xdr:nvPicPr>
+        <xdr:blipFill>
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+          <a:srcRect/>
+          <a:stretch>
+            <a:fillRect/>
+          </a:stretch>
+        </xdr:blipFill>
+        <xdr:spPr bwMode="auto">
+          <a:xfrm>
+            <a:off x="1338" y="2976"/>
+            <a:ext cx="456" cy="462"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln w="9525">
+            <a:noFill/>
+            <a:miter lim="800000"/>
+            <a:headEnd/>
+            <a:tailEnd/>
+          </a:ln>
+        </xdr:spPr>
+      </xdr:pic>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="9" name="Text Box 6"/>
+          <xdr:cNvSpPr txBox="1">
+            <a:spLocks noChangeArrowheads="1"/>
+          </xdr:cNvSpPr>
+        </xdr:nvSpPr>
+        <xdr:spPr bwMode="auto">
+          <a:xfrm>
+            <a:off x="1247" y="3430"/>
+            <a:ext cx="680" cy="192"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln w="9525">
+            <a:noFill/>
+            <a:miter lim="800000"/>
+            <a:headEnd/>
+            <a:tailEnd/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:txBody>
+          <a:bodyPr wrap="square">
+            <a:spAutoFit/>
+          </a:bodyPr>
+          <a:lstStyle>
+            <a:defPPr>
+              <a:defRPr lang="ko-KR"/>
+            </a:defPPr>
+            <a:lvl1pPr marL="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl1pPr>
+            <a:lvl2pPr marL="457200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl2pPr>
+            <a:lvl3pPr marL="914400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl3pPr>
+            <a:lvl4pPr marL="1371600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl4pPr>
+            <a:lvl5pPr marL="1828800" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl5pPr>
+            <a:lvl6pPr marL="2286000" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl6pPr>
+            <a:lvl7pPr marL="2743200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl7pPr>
+            <a:lvl8pPr marL="3200400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl8pPr>
+            <a:lvl9pPr marL="3657600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl9pPr>
+          </a:lstStyle>
+          <a:p>
+            <a:pPr>
+              <a:spcBef>
+                <a:spcPct val="50000"/>
+              </a:spcBef>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="ko-KR" altLang="en-US" sz="1400"/>
+              <a:t>클라이언트</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>195294</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>61912</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>266732</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>132862</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="10" name="Rectangle 5"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="4310094" y="1319212"/>
+          <a:ext cx="71438" cy="2376000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent1"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr wrap="square" anchor="ctr"/>
+        <a:lstStyle>
+          <a:defPPr>
+            <a:defRPr lang="ko-KR"/>
+          </a:defPPr>
+          <a:lvl1pPr marL="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p>
+          <a:endParaRPr lang="ko-KR" altLang="en-US"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>90490</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>153980</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>161924</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>153980</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="11" name="직선 화살표 연결선 10"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1462090" y="1830380"/>
+          <a:ext cx="2814634" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>90490</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>93662</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>180974</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>93662</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="12" name="직선 화살표 연결선 11"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="1462090" y="2398712"/>
+          <a:ext cx="2833684" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>161925</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>26213</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>200024</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>96868</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="13" name="Text Box 10"/>
+        <xdr:cNvSpPr txBox="1">
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="1533525" y="2121713"/>
+          <a:ext cx="1409699" cy="280205"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525">
+          <a:noFill/>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr wrap="square">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle>
+          <a:defPPr>
+            <a:defRPr lang="ko-KR"/>
+          </a:defPPr>
+          <a:lvl1pPr marL="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p>
+          <a:pPr>
+            <a:spcBef>
+              <a:spcPct val="50000"/>
+            </a:spcBef>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ko-KR" sz="1200"/>
+            <a:t>LOBBY_CHAT_RES</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="14" name="Group 4"/>
+        <xdr:cNvGrpSpPr>
+          <a:grpSpLocks/>
+        </xdr:cNvGrpSpPr>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="2667000"/>
+          <a:ext cx="1600200" cy="1123950"/>
+          <a:chOff x="1037" y="2976"/>
+          <a:chExt cx="1008" cy="708"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:pic>
+        <xdr:nvPicPr>
+          <xdr:cNvPr id="15" name="Picture 5"/>
+          <xdr:cNvPicPr>
+            <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+          </xdr:cNvPicPr>
+        </xdr:nvPicPr>
+        <xdr:blipFill>
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+          <a:srcRect/>
+          <a:stretch>
+            <a:fillRect/>
+          </a:stretch>
+        </xdr:blipFill>
+        <xdr:spPr bwMode="auto">
+          <a:xfrm>
+            <a:off x="1338" y="2976"/>
+            <a:ext cx="456" cy="462"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln w="9525">
+            <a:noFill/>
+            <a:miter lim="800000"/>
+            <a:headEnd/>
+            <a:tailEnd/>
+          </a:ln>
+        </xdr:spPr>
+      </xdr:pic>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="16" name="Text Box 6"/>
+          <xdr:cNvSpPr txBox="1">
+            <a:spLocks noChangeArrowheads="1"/>
+          </xdr:cNvSpPr>
+        </xdr:nvSpPr>
+        <xdr:spPr bwMode="auto">
+          <a:xfrm>
+            <a:off x="1037" y="3430"/>
+            <a:ext cx="1008" cy="254"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln w="9525">
+            <a:noFill/>
+            <a:miter lim="800000"/>
+            <a:headEnd/>
+            <a:tailEnd/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:txBody>
+          <a:bodyPr wrap="square">
+            <a:spAutoFit/>
+          </a:bodyPr>
+          <a:lstStyle>
+            <a:defPPr>
+              <a:defRPr lang="ko-KR"/>
+            </a:defPPr>
+            <a:lvl1pPr marL="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl1pPr>
+            <a:lvl2pPr marL="457200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl2pPr>
+            <a:lvl3pPr marL="914400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl3pPr>
+            <a:lvl4pPr marL="1371600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl4pPr>
+            <a:lvl5pPr marL="1828800" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl5pPr>
+            <a:lvl6pPr marL="2286000" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl6pPr>
+            <a:lvl7pPr marL="2743200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl7pPr>
+            <a:lvl8pPr marL="3200400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl8pPr>
+            <a:lvl9pPr marL="3657600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl9pPr>
+          </a:lstStyle>
+          <a:p>
+            <a:pPr>
+              <a:spcBef>
+                <a:spcPct val="50000"/>
+              </a:spcBef>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="ko-KR" altLang="en-US" sz="1400"/>
+              <a:t>로비의 다른 유저</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>609600</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>774</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>195259</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>774</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="17" name="직선 화살표 연결선 16"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="1295400" y="3353574"/>
+          <a:ext cx="3014659" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>52385</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>90484</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>3980</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="18" name="Text Box 10"/>
+        <xdr:cNvSpPr txBox="1">
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="1423985" y="3076575"/>
+          <a:ext cx="1409699" cy="280205"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525">
+          <a:noFill/>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr wrap="square">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle>
+          <a:defPPr>
+            <a:defRPr lang="ko-KR"/>
+          </a:defPPr>
+          <a:lvl1pPr marL="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p>
+          <a:pPr>
+            <a:spcBef>
+              <a:spcPct val="50000"/>
+            </a:spcBef>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ko-KR" sz="1200"/>
+            <a:t>LOBBY_CHAT_NTF</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>28578</xdr:colOff>
       <xdr:row>6</xdr:row>
       <xdr:rowOff>61912</xdr:rowOff>
@@ -2501,8 +5480,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr bwMode="auto">
         <a:xfrm>
-          <a:off x="3748115" y="315919"/>
-          <a:ext cx="1512887" cy="954090"/>
+          <a:off x="3748115" y="311156"/>
+          <a:ext cx="1512887" cy="935040"/>
           <a:chOff x="427" y="270"/>
           <a:chExt cx="91" cy="96"/>
         </a:xfrm>
@@ -2847,8 +5826,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr bwMode="auto">
         <a:xfrm>
-          <a:off x="971550" y="300038"/>
-          <a:ext cx="1079500" cy="1049337"/>
+          <a:off x="971550" y="295275"/>
+          <a:ext cx="1079500" cy="1025525"/>
           <a:chOff x="1247" y="2976"/>
           <a:chExt cx="680" cy="646"/>
         </a:xfrm>
@@ -3432,8 +6411,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr bwMode="auto">
         <a:xfrm>
-          <a:off x="0" y="2667000"/>
-          <a:ext cx="1600200" cy="1147763"/>
+          <a:off x="0" y="2609850"/>
+          <a:ext cx="1600200" cy="1123950"/>
           <a:chOff x="1037" y="2976"/>
           <a:chExt cx="1008" cy="708"/>
         </a:xfrm>
@@ -3885,7 +6864,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -4053,8 +7032,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr bwMode="auto">
         <a:xfrm>
-          <a:off x="3738590" y="315919"/>
-          <a:ext cx="1512887" cy="954090"/>
+          <a:off x="3738590" y="311156"/>
+          <a:ext cx="1512887" cy="935040"/>
           <a:chOff x="427" y="270"/>
           <a:chExt cx="91" cy="96"/>
         </a:xfrm>
@@ -4399,8 +7378,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr bwMode="auto">
         <a:xfrm>
-          <a:off x="962025" y="300038"/>
-          <a:ext cx="1079500" cy="1049337"/>
+          <a:off x="962025" y="295275"/>
+          <a:ext cx="1079500" cy="1025525"/>
           <a:chOff x="1247" y="2976"/>
           <a:chExt cx="680" cy="646"/>
         </a:xfrm>
@@ -5027,7 +8006,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -5195,8 +8174,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr bwMode="auto">
         <a:xfrm>
-          <a:off x="3738590" y="315919"/>
-          <a:ext cx="1512887" cy="954090"/>
+          <a:off x="3738590" y="311156"/>
+          <a:ext cx="1512887" cy="935040"/>
           <a:chOff x="427" y="270"/>
           <a:chExt cx="91" cy="96"/>
         </a:xfrm>
@@ -5541,8 +8520,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr bwMode="auto">
         <a:xfrm>
-          <a:off x="962025" y="300038"/>
-          <a:ext cx="1079500" cy="1049337"/>
+          <a:off x="962025" y="295275"/>
+          <a:ext cx="1079500" cy="1025525"/>
           <a:chOff x="1247" y="2976"/>
           <a:chExt cx="680" cy="646"/>
         </a:xfrm>
@@ -6169,7 +9148,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -7721,7 +10700,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing8.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -9864,7 +12843,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing9.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -11998,1480 +14977,6 @@
           <a:r>
             <a:rPr lang="en-US" altLang="ko-KR" sz="1200"/>
             <a:t>ROOM_CHANGED_INFO_NTF</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing9.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>19053</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>61913</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>90490</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>172613</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="14" name="Rectangle 5"/>
-        <xdr:cNvSpPr>
-          <a:spLocks noChangeArrowheads="1"/>
-        </xdr:cNvSpPr>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="1390653" y="1319213"/>
-          <a:ext cx="71437" cy="1368000"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="accent1"/>
-        </a:solidFill>
-        <a:ln w="9525">
-          <a:solidFill>
-            <a:schemeClr val="tx1"/>
-          </a:solidFill>
-          <a:miter lim="800000"/>
-          <a:headEnd/>
-          <a:tailEnd/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:txBody>
-        <a:bodyPr wrap="square" anchor="ctr"/>
-        <a:lstStyle>
-          <a:defPPr>
-            <a:defRPr lang="ko-KR"/>
-          </a:defPPr>
-          <a:lvl1pPr marL="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
-            <a:defRPr sz="1800" kern="1200">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl1pPr>
-          <a:lvl2pPr marL="457200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
-            <a:defRPr sz="1800" kern="1200">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl2pPr>
-          <a:lvl3pPr marL="914400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
-            <a:defRPr sz="1800" kern="1200">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl3pPr>
-          <a:lvl4pPr marL="1371600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
-            <a:defRPr sz="1800" kern="1200">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl4pPr>
-          <a:lvl5pPr marL="1828800" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
-            <a:defRPr sz="1800" kern="1200">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl5pPr>
-          <a:lvl6pPr marL="2286000" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
-            <a:defRPr sz="1800" kern="1200">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl6pPr>
-          <a:lvl7pPr marL="2743200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
-            <a:defRPr sz="1800" kern="1200">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl7pPr>
-          <a:lvl8pPr marL="3200400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
-            <a:defRPr sz="1800" kern="1200">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl8pPr>
-          <a:lvl9pPr marL="3657600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
-            <a:defRPr sz="1800" kern="1200">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl9pPr>
-        </a:lstStyle>
-        <a:p>
-          <a:endParaRPr lang="ko-KR" altLang="en-US"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>309590</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>101606</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>450877</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>198446</xdr:rowOff>
-    </xdr:to>
-    <xdr:grpSp>
-      <xdr:nvGrpSpPr>
-        <xdr:cNvPr id="15" name="Group 7"/>
-        <xdr:cNvGrpSpPr>
-          <a:grpSpLocks/>
-        </xdr:cNvGrpSpPr>
-      </xdr:nvGrpSpPr>
-      <xdr:grpSpPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="3738590" y="315919"/>
-          <a:ext cx="1512887" cy="954090"/>
-          <a:chOff x="427" y="270"/>
-          <a:chExt cx="91" cy="96"/>
-        </a:xfrm>
-      </xdr:grpSpPr>
-      <xdr:sp macro="" textlink="">
-        <xdr:nvSpPr>
-          <xdr:cNvPr id="16" name="Text Box 8"/>
-          <xdr:cNvSpPr txBox="1">
-            <a:spLocks noChangeArrowheads="1"/>
-          </xdr:cNvSpPr>
-        </xdr:nvSpPr>
-        <xdr:spPr bwMode="auto">
-          <a:xfrm>
-            <a:off x="429" y="345"/>
-            <a:ext cx="89" cy="21"/>
-          </a:xfrm>
-          <a:prstGeom prst="rect">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:solidFill>
-            <a:srgbClr val="FFFFFF"/>
-          </a:solidFill>
-          <a:ln w="9525">
-            <a:noFill/>
-            <a:miter lim="800000"/>
-            <a:headEnd/>
-            <a:tailEnd/>
-          </a:ln>
-        </xdr:spPr>
-        <xdr:txBody>
-          <a:bodyPr wrap="square"/>
-          <a:lstStyle>
-            <a:defPPr>
-              <a:defRPr lang="ko-KR"/>
-            </a:defPPr>
-            <a:lvl1pPr marL="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
-              <a:defRPr sz="1800" kern="1200">
-                <a:solidFill>
-                  <a:schemeClr val="tx1"/>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:lvl1pPr>
-            <a:lvl2pPr marL="457200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
-              <a:defRPr sz="1800" kern="1200">
-                <a:solidFill>
-                  <a:schemeClr val="tx1"/>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:lvl2pPr>
-            <a:lvl3pPr marL="914400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
-              <a:defRPr sz="1800" kern="1200">
-                <a:solidFill>
-                  <a:schemeClr val="tx1"/>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:lvl3pPr>
-            <a:lvl4pPr marL="1371600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
-              <a:defRPr sz="1800" kern="1200">
-                <a:solidFill>
-                  <a:schemeClr val="tx1"/>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:lvl4pPr>
-            <a:lvl5pPr marL="1828800" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
-              <a:defRPr sz="1800" kern="1200">
-                <a:solidFill>
-                  <a:schemeClr val="tx1"/>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:lvl5pPr>
-            <a:lvl6pPr marL="2286000" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
-              <a:defRPr sz="1800" kern="1200">
-                <a:solidFill>
-                  <a:schemeClr val="tx1"/>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:lvl6pPr>
-            <a:lvl7pPr marL="2743200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
-              <a:defRPr sz="1800" kern="1200">
-                <a:solidFill>
-                  <a:schemeClr val="tx1"/>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:lvl7pPr>
-            <a:lvl8pPr marL="3200400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
-              <a:defRPr sz="1800" kern="1200">
-                <a:solidFill>
-                  <a:schemeClr val="tx1"/>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:lvl8pPr>
-            <a:lvl9pPr marL="3657600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
-              <a:defRPr sz="1800" kern="1200">
-                <a:solidFill>
-                  <a:schemeClr val="tx1"/>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:lvl9pPr>
-          </a:lstStyle>
-          <a:p>
-            <a:r>
-              <a:rPr lang="en-US" altLang="ko-KR" sz="1200"/>
-              <a:t>   </a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="ko-KR" altLang="en-US" sz="1200"/>
-              <a:t>채팅 서버</a:t>
-            </a:r>
-          </a:p>
-        </xdr:txBody>
-      </xdr:sp>
-      <xdr:pic>
-        <xdr:nvPicPr>
-          <xdr:cNvPr id="17" name="Picture 9"/>
-          <xdr:cNvPicPr>
-            <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-          </xdr:cNvPicPr>
-        </xdr:nvPicPr>
-        <xdr:blipFill>
-          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
-          <a:srcRect/>
-          <a:stretch>
-            <a:fillRect/>
-          </a:stretch>
-        </xdr:blipFill>
-        <xdr:spPr bwMode="auto">
-          <a:xfrm>
-            <a:off x="427" y="270"/>
-            <a:ext cx="78" cy="78"/>
-          </a:xfrm>
-          <a:prstGeom prst="rect">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:noFill/>
-          <a:ln w="9525">
-            <a:noFill/>
-            <a:miter lim="800000"/>
-            <a:headEnd/>
-            <a:tailEnd/>
-          </a:ln>
-        </xdr:spPr>
-      </xdr:pic>
-    </xdr:grpSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>104776</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>107941</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>228600</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>178596</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="18" name="Text Box 10"/>
-        <xdr:cNvSpPr txBox="1">
-          <a:spLocks noChangeArrowheads="1"/>
-        </xdr:cNvSpPr>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="2847976" y="1574791"/>
-          <a:ext cx="1495424" cy="280205"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln w="9525">
-          <a:noFill/>
-          <a:miter lim="800000"/>
-          <a:headEnd/>
-          <a:tailEnd/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:txBody>
-        <a:bodyPr wrap="square">
-          <a:spAutoFit/>
-        </a:bodyPr>
-        <a:lstStyle>
-          <a:defPPr>
-            <a:defRPr lang="ko-KR"/>
-          </a:defPPr>
-          <a:lvl1pPr marL="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
-            <a:defRPr sz="1800" kern="1200">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl1pPr>
-          <a:lvl2pPr marL="457200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
-            <a:defRPr sz="1800" kern="1200">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl2pPr>
-          <a:lvl3pPr marL="914400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
-            <a:defRPr sz="1800" kern="1200">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl3pPr>
-          <a:lvl4pPr marL="1371600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
-            <a:defRPr sz="1800" kern="1200">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl4pPr>
-          <a:lvl5pPr marL="1828800" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
-            <a:defRPr sz="1800" kern="1200">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl5pPr>
-          <a:lvl6pPr marL="2286000" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
-            <a:defRPr sz="1800" kern="1200">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl6pPr>
-          <a:lvl7pPr marL="2743200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
-            <a:defRPr sz="1800" kern="1200">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl7pPr>
-          <a:lvl8pPr marL="3200400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
-            <a:defRPr sz="1800" kern="1200">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl8pPr>
-          <a:lvl9pPr marL="3657600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
-            <a:defRPr sz="1800" kern="1200">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl9pPr>
-        </a:lstStyle>
-        <a:p>
-          <a:pPr>
-            <a:spcBef>
-              <a:spcPct val="50000"/>
-            </a:spcBef>
-          </a:pPr>
-          <a:r>
-            <a:rPr lang="en-US" altLang="ko-KR" sz="1200"/>
-            <a:t>ROOM_CHAT_REQ</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>276225</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>669925</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>63500</xdr:rowOff>
-    </xdr:to>
-    <xdr:grpSp>
-      <xdr:nvGrpSpPr>
-        <xdr:cNvPr id="19" name="Group 4"/>
-        <xdr:cNvGrpSpPr>
-          <a:grpSpLocks/>
-        </xdr:cNvGrpSpPr>
-      </xdr:nvGrpSpPr>
-      <xdr:grpSpPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="962025" y="300038"/>
-          <a:ext cx="1079500" cy="1049337"/>
-          <a:chOff x="1247" y="2976"/>
-          <a:chExt cx="680" cy="646"/>
-        </a:xfrm>
-      </xdr:grpSpPr>
-      <xdr:pic>
-        <xdr:nvPicPr>
-          <xdr:cNvPr id="20" name="Picture 5"/>
-          <xdr:cNvPicPr>
-            <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-          </xdr:cNvPicPr>
-        </xdr:nvPicPr>
-        <xdr:blipFill>
-          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
-          <a:srcRect/>
-          <a:stretch>
-            <a:fillRect/>
-          </a:stretch>
-        </xdr:blipFill>
-        <xdr:spPr bwMode="auto">
-          <a:xfrm>
-            <a:off x="1338" y="2976"/>
-            <a:ext cx="456" cy="462"/>
-          </a:xfrm>
-          <a:prstGeom prst="rect">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:noFill/>
-          <a:ln w="9525">
-            <a:noFill/>
-            <a:miter lim="800000"/>
-            <a:headEnd/>
-            <a:tailEnd/>
-          </a:ln>
-        </xdr:spPr>
-      </xdr:pic>
-      <xdr:sp macro="" textlink="">
-        <xdr:nvSpPr>
-          <xdr:cNvPr id="21" name="Text Box 6"/>
-          <xdr:cNvSpPr txBox="1">
-            <a:spLocks noChangeArrowheads="1"/>
-          </xdr:cNvSpPr>
-        </xdr:nvSpPr>
-        <xdr:spPr bwMode="auto">
-          <a:xfrm>
-            <a:off x="1247" y="3430"/>
-            <a:ext cx="680" cy="192"/>
-          </a:xfrm>
-          <a:prstGeom prst="rect">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:noFill/>
-          <a:ln w="9525">
-            <a:noFill/>
-            <a:miter lim="800000"/>
-            <a:headEnd/>
-            <a:tailEnd/>
-          </a:ln>
-        </xdr:spPr>
-        <xdr:txBody>
-          <a:bodyPr wrap="square">
-            <a:spAutoFit/>
-          </a:bodyPr>
-          <a:lstStyle>
-            <a:defPPr>
-              <a:defRPr lang="ko-KR"/>
-            </a:defPPr>
-            <a:lvl1pPr marL="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
-              <a:defRPr sz="1800" kern="1200">
-                <a:solidFill>
-                  <a:schemeClr val="tx1"/>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:lvl1pPr>
-            <a:lvl2pPr marL="457200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
-              <a:defRPr sz="1800" kern="1200">
-                <a:solidFill>
-                  <a:schemeClr val="tx1"/>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:lvl2pPr>
-            <a:lvl3pPr marL="914400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
-              <a:defRPr sz="1800" kern="1200">
-                <a:solidFill>
-                  <a:schemeClr val="tx1"/>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:lvl3pPr>
-            <a:lvl4pPr marL="1371600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
-              <a:defRPr sz="1800" kern="1200">
-                <a:solidFill>
-                  <a:schemeClr val="tx1"/>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:lvl4pPr>
-            <a:lvl5pPr marL="1828800" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
-              <a:defRPr sz="1800" kern="1200">
-                <a:solidFill>
-                  <a:schemeClr val="tx1"/>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:lvl5pPr>
-            <a:lvl6pPr marL="2286000" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
-              <a:defRPr sz="1800" kern="1200">
-                <a:solidFill>
-                  <a:schemeClr val="tx1"/>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:lvl6pPr>
-            <a:lvl7pPr marL="2743200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
-              <a:defRPr sz="1800" kern="1200">
-                <a:solidFill>
-                  <a:schemeClr val="tx1"/>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:lvl7pPr>
-            <a:lvl8pPr marL="3200400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
-              <a:defRPr sz="1800" kern="1200">
-                <a:solidFill>
-                  <a:schemeClr val="tx1"/>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:lvl8pPr>
-            <a:lvl9pPr marL="3657600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
-              <a:defRPr sz="1800" kern="1200">
-                <a:solidFill>
-                  <a:schemeClr val="tx1"/>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:lvl9pPr>
-          </a:lstStyle>
-          <a:p>
-            <a:pPr>
-              <a:spcBef>
-                <a:spcPct val="50000"/>
-              </a:spcBef>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="ko-KR" altLang="en-US" sz="1400"/>
-              <a:t>클라이언트</a:t>
-            </a:r>
-          </a:p>
-        </xdr:txBody>
-      </xdr:sp>
-    </xdr:grpSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>195294</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>61912</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>266732</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>132862</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="22" name="Rectangle 5"/>
-        <xdr:cNvSpPr>
-          <a:spLocks noChangeArrowheads="1"/>
-        </xdr:cNvSpPr>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="4310094" y="1319212"/>
-          <a:ext cx="71438" cy="2376000"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="accent1"/>
-        </a:solidFill>
-        <a:ln w="9525">
-          <a:solidFill>
-            <a:schemeClr val="tx1"/>
-          </a:solidFill>
-          <a:miter lim="800000"/>
-          <a:headEnd/>
-          <a:tailEnd/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:txBody>
-        <a:bodyPr wrap="square" anchor="ctr"/>
-        <a:lstStyle>
-          <a:defPPr>
-            <a:defRPr lang="ko-KR"/>
-          </a:defPPr>
-          <a:lvl1pPr marL="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
-            <a:defRPr sz="1800" kern="1200">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl1pPr>
-          <a:lvl2pPr marL="457200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
-            <a:defRPr sz="1800" kern="1200">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl2pPr>
-          <a:lvl3pPr marL="914400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
-            <a:defRPr sz="1800" kern="1200">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl3pPr>
-          <a:lvl4pPr marL="1371600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
-            <a:defRPr sz="1800" kern="1200">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl4pPr>
-          <a:lvl5pPr marL="1828800" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
-            <a:defRPr sz="1800" kern="1200">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl5pPr>
-          <a:lvl6pPr marL="2286000" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
-            <a:defRPr sz="1800" kern="1200">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl6pPr>
-          <a:lvl7pPr marL="2743200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
-            <a:defRPr sz="1800" kern="1200">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl7pPr>
-          <a:lvl8pPr marL="3200400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
-            <a:defRPr sz="1800" kern="1200">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl8pPr>
-          <a:lvl9pPr marL="3657600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
-            <a:defRPr sz="1800" kern="1200">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl9pPr>
-        </a:lstStyle>
-        <a:p>
-          <a:endParaRPr lang="ko-KR" altLang="en-US"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>90490</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>153980</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>161924</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>153980</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="23" name="직선 화살표 연결선 22"/>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="1462090" y="1830380"/>
-          <a:ext cx="2814634" cy="0"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:tailEnd type="arrow"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="dk1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>90490</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>93662</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>180974</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>93662</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="24" name="직선 화살표 연결선 23"/>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipH="1">
-          <a:off x="1462090" y="2398712"/>
-          <a:ext cx="2833684" cy="0"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:tailEnd type="arrow"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="dk1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>161925</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>26213</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>200024</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>96868</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="25" name="Text Box 10"/>
-        <xdr:cNvSpPr txBox="1">
-          <a:spLocks noChangeArrowheads="1"/>
-        </xdr:cNvSpPr>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="1533525" y="2121713"/>
-          <a:ext cx="1409699" cy="280205"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln w="9525">
-          <a:noFill/>
-          <a:miter lim="800000"/>
-          <a:headEnd/>
-          <a:tailEnd/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:txBody>
-        <a:bodyPr wrap="square">
-          <a:spAutoFit/>
-        </a:bodyPr>
-        <a:lstStyle>
-          <a:defPPr>
-            <a:defRPr lang="ko-KR"/>
-          </a:defPPr>
-          <a:lvl1pPr marL="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
-            <a:defRPr sz="1800" kern="1200">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl1pPr>
-          <a:lvl2pPr marL="457200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
-            <a:defRPr sz="1800" kern="1200">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl2pPr>
-          <a:lvl3pPr marL="914400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
-            <a:defRPr sz="1800" kern="1200">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl3pPr>
-          <a:lvl4pPr marL="1371600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
-            <a:defRPr sz="1800" kern="1200">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl4pPr>
-          <a:lvl5pPr marL="1828800" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
-            <a:defRPr sz="1800" kern="1200">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl5pPr>
-          <a:lvl6pPr marL="2286000" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
-            <a:defRPr sz="1800" kern="1200">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl6pPr>
-          <a:lvl7pPr marL="2743200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
-            <a:defRPr sz="1800" kern="1200">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl7pPr>
-          <a:lvl8pPr marL="3200400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
-            <a:defRPr sz="1800" kern="1200">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl8pPr>
-          <a:lvl9pPr marL="3657600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
-            <a:defRPr sz="1800" kern="1200">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl9pPr>
-        </a:lstStyle>
-        <a:p>
-          <a:pPr>
-            <a:spcBef>
-              <a:spcPct val="50000"/>
-            </a:spcBef>
-          </a:pPr>
-          <a:r>
-            <a:rPr lang="en-US" altLang="ko-KR" sz="1200"/>
-            <a:t>ROOM_CHAT_RES</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>228600</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
-    </xdr:to>
-    <xdr:grpSp>
-      <xdr:nvGrpSpPr>
-        <xdr:cNvPr id="26" name="Group 4"/>
-        <xdr:cNvGrpSpPr>
-          <a:grpSpLocks/>
-        </xdr:cNvGrpSpPr>
-      </xdr:nvGrpSpPr>
-      <xdr:grpSpPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="0" y="2724150"/>
-          <a:ext cx="1600200" cy="1152525"/>
-          <a:chOff x="1037" y="2976"/>
-          <a:chExt cx="1008" cy="708"/>
-        </a:xfrm>
-      </xdr:grpSpPr>
-      <xdr:pic>
-        <xdr:nvPicPr>
-          <xdr:cNvPr id="27" name="Picture 5"/>
-          <xdr:cNvPicPr>
-            <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-          </xdr:cNvPicPr>
-        </xdr:nvPicPr>
-        <xdr:blipFill>
-          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
-          <a:srcRect/>
-          <a:stretch>
-            <a:fillRect/>
-          </a:stretch>
-        </xdr:blipFill>
-        <xdr:spPr bwMode="auto">
-          <a:xfrm>
-            <a:off x="1338" y="2976"/>
-            <a:ext cx="456" cy="462"/>
-          </a:xfrm>
-          <a:prstGeom prst="rect">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:noFill/>
-          <a:ln w="9525">
-            <a:noFill/>
-            <a:miter lim="800000"/>
-            <a:headEnd/>
-            <a:tailEnd/>
-          </a:ln>
-        </xdr:spPr>
-      </xdr:pic>
-      <xdr:sp macro="" textlink="">
-        <xdr:nvSpPr>
-          <xdr:cNvPr id="28" name="Text Box 6"/>
-          <xdr:cNvSpPr txBox="1">
-            <a:spLocks noChangeArrowheads="1"/>
-          </xdr:cNvSpPr>
-        </xdr:nvSpPr>
-        <xdr:spPr bwMode="auto">
-          <a:xfrm>
-            <a:off x="1037" y="3430"/>
-            <a:ext cx="1008" cy="254"/>
-          </a:xfrm>
-          <a:prstGeom prst="rect">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:noFill/>
-          <a:ln w="9525">
-            <a:noFill/>
-            <a:miter lim="800000"/>
-            <a:headEnd/>
-            <a:tailEnd/>
-          </a:ln>
-        </xdr:spPr>
-        <xdr:txBody>
-          <a:bodyPr wrap="square">
-            <a:spAutoFit/>
-          </a:bodyPr>
-          <a:lstStyle>
-            <a:defPPr>
-              <a:defRPr lang="ko-KR"/>
-            </a:defPPr>
-            <a:lvl1pPr marL="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
-              <a:defRPr sz="1800" kern="1200">
-                <a:solidFill>
-                  <a:schemeClr val="tx1"/>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:lvl1pPr>
-            <a:lvl2pPr marL="457200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
-              <a:defRPr sz="1800" kern="1200">
-                <a:solidFill>
-                  <a:schemeClr val="tx1"/>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:lvl2pPr>
-            <a:lvl3pPr marL="914400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
-              <a:defRPr sz="1800" kern="1200">
-                <a:solidFill>
-                  <a:schemeClr val="tx1"/>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:lvl3pPr>
-            <a:lvl4pPr marL="1371600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
-              <a:defRPr sz="1800" kern="1200">
-                <a:solidFill>
-                  <a:schemeClr val="tx1"/>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:lvl4pPr>
-            <a:lvl5pPr marL="1828800" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
-              <a:defRPr sz="1800" kern="1200">
-                <a:solidFill>
-                  <a:schemeClr val="tx1"/>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:lvl5pPr>
-            <a:lvl6pPr marL="2286000" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
-              <a:defRPr sz="1800" kern="1200">
-                <a:solidFill>
-                  <a:schemeClr val="tx1"/>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:lvl6pPr>
-            <a:lvl7pPr marL="2743200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
-              <a:defRPr sz="1800" kern="1200">
-                <a:solidFill>
-                  <a:schemeClr val="tx1"/>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:lvl7pPr>
-            <a:lvl8pPr marL="3200400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
-              <a:defRPr sz="1800" kern="1200">
-                <a:solidFill>
-                  <a:schemeClr val="tx1"/>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:lvl8pPr>
-            <a:lvl9pPr marL="3657600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
-              <a:defRPr sz="1800" kern="1200">
-                <a:solidFill>
-                  <a:schemeClr val="tx1"/>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:lvl9pPr>
-          </a:lstStyle>
-          <a:p>
-            <a:pPr>
-              <a:spcBef>
-                <a:spcPct val="50000"/>
-              </a:spcBef>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="ko-KR" altLang="en-US" sz="1400"/>
-              <a:t>방의 다른 유저</a:t>
-            </a:r>
-          </a:p>
-        </xdr:txBody>
-      </xdr:sp>
-    </xdr:grpSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>609600</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>774</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>195259</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>774</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="29" name="직선 화살표 연결선 28"/>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipH="1">
-          <a:off x="1295400" y="3353574"/>
-          <a:ext cx="3014659" cy="0"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:tailEnd type="arrow"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="dk1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>52385</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>90484</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>3980</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="30" name="Text Box 10"/>
-        <xdr:cNvSpPr txBox="1">
-          <a:spLocks noChangeArrowheads="1"/>
-        </xdr:cNvSpPr>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="1423985" y="3076575"/>
-          <a:ext cx="1409699" cy="280205"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln w="9525">
-          <a:noFill/>
-          <a:miter lim="800000"/>
-          <a:headEnd/>
-          <a:tailEnd/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:txBody>
-        <a:bodyPr wrap="square">
-          <a:spAutoFit/>
-        </a:bodyPr>
-        <a:lstStyle>
-          <a:defPPr>
-            <a:defRPr lang="ko-KR"/>
-          </a:defPPr>
-          <a:lvl1pPr marL="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
-            <a:defRPr sz="1800" kern="1200">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl1pPr>
-          <a:lvl2pPr marL="457200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
-            <a:defRPr sz="1800" kern="1200">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl2pPr>
-          <a:lvl3pPr marL="914400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
-            <a:defRPr sz="1800" kern="1200">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl3pPr>
-          <a:lvl4pPr marL="1371600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
-            <a:defRPr sz="1800" kern="1200">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl4pPr>
-          <a:lvl5pPr marL="1828800" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
-            <a:defRPr sz="1800" kern="1200">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl5pPr>
-          <a:lvl6pPr marL="2286000" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
-            <a:defRPr sz="1800" kern="1200">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl6pPr>
-          <a:lvl7pPr marL="2743200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
-            <a:defRPr sz="1800" kern="1200">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl7pPr>
-          <a:lvl8pPr marL="3200400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
-            <a:defRPr sz="1800" kern="1200">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl8pPr>
-          <a:lvl9pPr marL="3657600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
-            <a:defRPr sz="1800" kern="1200">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl9pPr>
-        </a:lstStyle>
-        <a:p>
-          <a:pPr>
-            <a:spcBef>
-              <a:spcPct val="50000"/>
-            </a:spcBef>
-          </a:pPr>
-          <a:r>
-            <a:rPr lang="en-US" altLang="ko-KR" sz="1200"/>
-            <a:t>ROOM_CHAT_NTF</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -13784,7 +15289,55 @@
       <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.899999999999999" x14ac:dyDescent="0.6"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F27" sqref="F27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F26" sqref="F26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -13800,7 +15353,7 @@
       <selection activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.899999999999999" x14ac:dyDescent="0.6"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -13812,11 +15365,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.899999999999999" x14ac:dyDescent="0.6"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -13828,9 +15381,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I16" sqref="I16"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.899999999999999" x14ac:dyDescent="0.6"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -13842,11 +15397,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.899999999999999" x14ac:dyDescent="0.6"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -13859,10 +15412,10 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J18" sqref="J18"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.899999999999999" x14ac:dyDescent="0.6"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -13874,15 +15427,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.899999999999999" x14ac:dyDescent="0.6"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -13890,15 +15440,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.899999999999999" x14ac:dyDescent="0.6"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -13907,10 +15454,10 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.899999999999999" x14ac:dyDescent="0.6"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>